<commit_message>
After making the Klp and Kmct1 negligible, the trends show promise besides outlier fits
</commit_message>
<xml_diff>
--- a/AICothersolutionbcrm.xlsx
+++ b/AICothersolutionbcrm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ADD474-5AE1-40EA-94A8-16AC397F35F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B2F886-DB4A-4049-B857-B4A91092781A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{AE6A6178-0E2E-4DD2-82C9-C1F9B1F5F6F6}"/>
   </bookViews>
@@ -387,178 +387,178 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>2252.9138844698396</v>
+        <v>2253.0781067697317</v>
       </c>
       <c r="B1">
-        <v>1484.011487518525</v>
+        <v>1483.9685362968162</v>
       </c>
       <c r="C1">
-        <v>1458.5264437184162</v>
+        <v>1458.5133411192824</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2245.4544140193943</v>
+        <v>2245.6994696923975</v>
       </c>
       <c r="B2">
-        <v>1472.0876637241449</v>
+        <v>1472.1466793336142</v>
       </c>
       <c r="C2">
-        <v>1381.4318171538414</v>
+        <v>1381.445659344791</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2336.4524007573832</v>
+        <v>2336.3606539419861</v>
       </c>
       <c r="B3">
-        <v>1616.6474568954643</v>
+        <v>1617.3803243389798</v>
       </c>
       <c r="C3">
-        <v>1522.5808236455223</v>
+        <v>1523.6429521765792</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2342.6416962808325</v>
+        <v>2342.6959957354397</v>
       </c>
       <c r="B4">
-        <v>1761.0773756089902</v>
+        <v>1760.9917129372232</v>
       </c>
       <c r="C4">
-        <v>1689.0097300275622</v>
+        <v>1688.7842662742169</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2434.0258564243263</v>
+        <v>2434.0838536611682</v>
       </c>
       <c r="B5">
-        <v>1672.2673289734701</v>
+        <v>1672.2771935457395</v>
       </c>
       <c r="C5">
-        <v>1684.3615484594504</v>
+        <v>1684.3558753920149</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2390.5578884586052</v>
+        <v>2391.5087082003142</v>
       </c>
       <c r="B6">
-        <v>1800.7217221654178</v>
+        <v>1800.8263427874533</v>
       </c>
       <c r="C6">
-        <v>1844.2000267710271</v>
+        <v>1844.1686302289995</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2137.6459970807418</v>
+        <v>2137.6359753035094</v>
       </c>
       <c r="B7">
-        <v>1574.9799446142638</v>
+        <v>1574.97839887856</v>
       </c>
       <c r="C7">
-        <v>1496.8283642768247</v>
+        <v>1496.8253296032933</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2229.136437827141</v>
+        <v>2229.1398539127986</v>
       </c>
       <c r="B8">
-        <v>1669.8607669298456</v>
+        <v>1669.8605423997008</v>
       </c>
       <c r="C8">
-        <v>1623.935345590035</v>
+        <v>1623.9368661733431</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2482.2397217020316</v>
+        <v>2482.2402730105773</v>
       </c>
       <c r="B9">
-        <v>1785.8680663214136</v>
+        <v>1785.8681603700272</v>
       </c>
       <c r="C9">
-        <v>1532.2375526789237</v>
+        <v>1532.2375750561569</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2137.6870870753196</v>
+        <v>2138.0482163449992</v>
       </c>
       <c r="B10">
-        <v>1367.6041988828192</v>
+        <v>1367.6533299098276</v>
       </c>
       <c r="C10">
-        <v>1355.2254120896521</v>
+        <v>1355.2378885605074</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>1914.3726505814341</v>
+        <v>1916.8469566312344</v>
       </c>
       <c r="B11">
-        <v>1487.3148561337578</v>
+        <v>1487.2807126562468</v>
       </c>
       <c r="C11">
-        <v>1340.3778694219848</v>
+        <v>1340.4127127280185</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2622.1838623628391</v>
+        <v>2622.0584919597882</v>
       </c>
       <c r="B12">
-        <v>2213.3837441749488</v>
+        <v>2213.368834647898</v>
       </c>
       <c r="C12">
-        <v>2008.1269833733973</v>
+        <v>2008.1358220437296</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2434.1559635630501</v>
+        <v>2434.133213466529</v>
       </c>
       <c r="B13">
-        <v>1771.7272666743613</v>
+        <v>1771.9811371311253</v>
       </c>
       <c r="C13">
-        <v>1801.8684438694327</v>
+        <v>1801.4379402012935</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>2533.5907965780916</v>
+        <v>2533.7957667574165</v>
       </c>
       <c r="B14">
-        <v>1892.5739411940729</v>
+        <v>1892.6393886710041</v>
       </c>
       <c r="C14">
-        <v>1676.6349946045873</v>
+        <v>1677.4589980148307</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>2608.6365938150639</v>
+        <v>2608.6706659603346</v>
       </c>
       <c r="B15">
-        <v>2053.7659067143509</v>
+        <v>2053.8989509474804</v>
       </c>
       <c r="C15">
-        <v>1937.5777493564062</v>
+        <v>1934.8879362898433</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>2246.9919232660518</v>
+        <v>2247.0020728089603</v>
       </c>
       <c r="B16">
-        <v>1531.9664790285926</v>
+        <v>1531.9965581307767</v>
       </c>
       <c r="C16">
-        <v>1286.2760683593274</v>
+        <v>1285.6448235637704</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Results of smoothing pyruvate: Didn't Change much at all
</commit_message>
<xml_diff>
--- a/AICothersolutionbcrm.xlsx
+++ b/AICothersolutionbcrm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B2F886-DB4A-4049-B857-B4A91092781A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C187FB-B755-453F-8525-83134FE56990}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{AE6A6178-0E2E-4DD2-82C9-C1F9B1F5F6F6}"/>
   </bookViews>
@@ -387,178 +387,178 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>2253.0781067697317</v>
+        <v>2252.8769924332587</v>
       </c>
       <c r="B1">
-        <v>1483.9685362968162</v>
+        <v>1484.0033959713637</v>
       </c>
       <c r="C1">
-        <v>1458.5133411192824</v>
+        <v>1458.5275370433824</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2245.6994696923975</v>
+        <v>2245.4342908856779</v>
       </c>
       <c r="B2">
-        <v>1472.1466793336142</v>
+        <v>1472.1372459917036</v>
       </c>
       <c r="C2">
-        <v>1381.445659344791</v>
+        <v>1381.4778522785523</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2336.3606539419861</v>
+        <v>2336.2597420911452</v>
       </c>
       <c r="B3">
-        <v>1617.3803243389798</v>
+        <v>1617.3939390796734</v>
       </c>
       <c r="C3">
-        <v>1523.6429521765792</v>
+        <v>1523.6787002040601</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2342.6959957354397</v>
+        <v>2342.6384360082379</v>
       </c>
       <c r="B4">
-        <v>1760.9917129372232</v>
+        <v>1760.881485260961</v>
       </c>
       <c r="C4">
-        <v>1688.7842662742169</v>
+        <v>1688.5508296593762</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2434.0838536611682</v>
+        <v>2433.9972554573974</v>
       </c>
       <c r="B5">
-        <v>1672.2771935457395</v>
+        <v>1672.2637748915399</v>
       </c>
       <c r="C5">
-        <v>1684.3558753920149</v>
+        <v>1684.3631976851311</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2391.5087082003142</v>
+        <v>2391.5474948084852</v>
       </c>
       <c r="B6">
-        <v>1800.8263427874533</v>
+        <v>1800.8304825546375</v>
       </c>
       <c r="C6">
-        <v>1844.1686302289995</v>
+        <v>1844.1674089106373</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2137.6359753035094</v>
+        <v>2137.5801402189309</v>
       </c>
       <c r="B7">
-        <v>1574.97839887856</v>
+        <v>1575.0429928910173</v>
       </c>
       <c r="C7">
-        <v>1496.8253296032933</v>
+        <v>1496.9727176723102</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2229.1398539127986</v>
+        <v>2229.0567285768507</v>
       </c>
       <c r="B8">
-        <v>1669.8605423997008</v>
+        <v>1669.8655607776607</v>
       </c>
       <c r="C8">
-        <v>1623.9368661733431</v>
+        <v>1623.9004324548439</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2482.2402730105773</v>
+        <v>2482.196155402482</v>
       </c>
       <c r="B9">
-        <v>1785.8681603700272</v>
+        <v>1785.8606392082324</v>
       </c>
       <c r="C9">
-        <v>1532.2375750561569</v>
+        <v>1532.2357883055745</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2138.0482163449992</v>
+        <v>2137.6540646913345</v>
       </c>
       <c r="B10">
-        <v>1367.6533299098276</v>
+        <v>1367.5997893964714</v>
       </c>
       <c r="C10">
-        <v>1355.2378885605074</v>
+        <v>1355.2241916899443</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>1916.8469566312344</v>
+        <v>1916.8392728789784</v>
       </c>
       <c r="B11">
-        <v>1487.2807126562468</v>
+        <v>1487.2801108329888</v>
       </c>
       <c r="C11">
-        <v>1340.4127127280185</v>
+        <v>1340.4166950075416</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2622.0584919597882</v>
+        <v>2622.1826605465953</v>
       </c>
       <c r="B12">
-        <v>2213.368834647898</v>
+        <v>2213.3836011013732</v>
       </c>
       <c r="C12">
-        <v>2008.1358220437296</v>
+        <v>2008.1270680731905</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2434.133213466529</v>
+        <v>2434.09136850499</v>
       </c>
       <c r="B13">
-        <v>1771.9811371311253</v>
+        <v>1771.8785422185199</v>
       </c>
       <c r="C13">
-        <v>1801.4379402012935</v>
+        <v>1801.6089744600852</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>2533.7957667574165</v>
+        <v>2533.9001931274552</v>
       </c>
       <c r="B14">
-        <v>1892.6393886710041</v>
+        <v>1892.7111131960464</v>
       </c>
       <c r="C14">
-        <v>1677.4589980148307</v>
+        <v>1678.8112363555049</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>2608.6706659603346</v>
+        <v>2609.2401229112861</v>
       </c>
       <c r="B15">
-        <v>2053.8989509474804</v>
+        <v>2053.9282352566352</v>
       </c>
       <c r="C15">
-        <v>1934.8879362898433</v>
+        <v>1936.1043017785341</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>2247.0020728089603</v>
+        <v>2247.0698900004686</v>
       </c>
       <c r="B16">
-        <v>1531.9965581307767</v>
+        <v>1531.9955049925056</v>
       </c>
       <c r="C16">
-        <v>1285.6448235637704</v>
+        <v>1285.6430914878229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ran With Different Bounds, Not Continuing Down this path
</commit_message>
<xml_diff>
--- a/AICothersolutionbcrm.xlsx
+++ b/AICothersolutionbcrm.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C187FB-B755-453F-8525-83134FE56990}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FF467E-C398-46DE-B8EA-C566F0225091}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{AE6A6178-0E2E-4DD2-82C9-C1F9B1F5F6F6}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{AE6A6178-0E2E-4DD2-82C9-C1F9B1F5F6F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -383,182 +383,182 @@
       <selection sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2252.8769924332587</v>
+        <v>2253.0246659930554</v>
       </c>
       <c r="B1">
-        <v>1484.0033959713637</v>
+        <v>1484.5375104173265</v>
       </c>
       <c r="C1">
-        <v>1458.5275370433824</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1458.5736134654164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2245.4342908856779</v>
+        <v>2245.2662449656004</v>
       </c>
       <c r="B2">
-        <v>1472.1372459917036</v>
+        <v>1471.2404910463865</v>
       </c>
       <c r="C2">
-        <v>1381.4778522785523</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1380.7460134102278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2336.2597420911452</v>
+        <v>2336.1676700863045</v>
       </c>
       <c r="B3">
-        <v>1617.3939390796734</v>
+        <v>1617.0565113740436</v>
       </c>
       <c r="C3">
-        <v>1523.6787002040601</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1523.1838345469969</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2342.6384360082379</v>
+        <v>2342.9978193578449</v>
       </c>
       <c r="B4">
-        <v>1760.881485260961</v>
+        <v>1761.5124566489699</v>
       </c>
       <c r="C4">
-        <v>1688.5508296593762</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1689.8979045080016</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2433.9972554573974</v>
+        <v>2434.1217742752733</v>
       </c>
       <c r="B5">
-        <v>1672.2637748915399</v>
+        <v>1672.2818283659492</v>
       </c>
       <c r="C5">
-        <v>1684.3631976851311</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1684.3537791446468</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2391.5474948084852</v>
+        <v>2391.6738806367443</v>
       </c>
       <c r="B6">
-        <v>1800.8304825546375</v>
+        <v>1801.4606032007052</v>
       </c>
       <c r="C6">
-        <v>1844.1674089106373</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1844.3669383967613</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2137.5801402189309</v>
+        <v>2137.565899469203</v>
       </c>
       <c r="B7">
-        <v>1575.0429928910173</v>
+        <v>1574.3978801186047</v>
       </c>
       <c r="C7">
-        <v>1496.9727176723102</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1495.5658458013481</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2229.0567285768507</v>
+        <v>2229.037756518248</v>
       </c>
       <c r="B8">
-        <v>1669.8655607776607</v>
+        <v>1669.9262810187711</v>
       </c>
       <c r="C8">
-        <v>1623.9004324548439</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1623.2863319398716</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2482.196155402482</v>
+        <v>2482.1508319710756</v>
       </c>
       <c r="B9">
-        <v>1785.8606392082324</v>
+        <v>1785.8529223760083</v>
       </c>
       <c r="C9">
-        <v>1532.2357883055745</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1532.2339656633517</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2137.6540646913345</v>
+        <v>2137.6608258863239</v>
       </c>
       <c r="B10">
-        <v>1367.5997893964714</v>
+        <v>1367.6007277853821</v>
       </c>
       <c r="C10">
-        <v>1355.2241916899443</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1355.2244003357537</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1916.8392728789784</v>
+        <v>1916.785965067352</v>
       </c>
       <c r="B11">
-        <v>1487.2801108329888</v>
+        <v>1487.2775584793419</v>
       </c>
       <c r="C11">
-        <v>1340.4166950075416</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1340.4566603589826</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2622.1826605465953</v>
+        <v>2624.0696799211869</v>
       </c>
       <c r="B12">
-        <v>2213.3836011013732</v>
+        <v>2214.4940293367436</v>
       </c>
       <c r="C12">
-        <v>2008.1270680731905</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2007.622886469951</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2434.09136850499</v>
+        <v>2434.1640767591011</v>
       </c>
       <c r="B13">
-        <v>1771.8785422185199</v>
+        <v>1772.1942831992394</v>
       </c>
       <c r="C13">
-        <v>1801.6089744600852</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1801.0800102327964</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2533.9001931274552</v>
+        <v>2533.7209044577908</v>
       </c>
       <c r="B14">
-        <v>1892.7111131960464</v>
+        <v>1892.4211717170908</v>
       </c>
       <c r="C14">
-        <v>1678.8112363555049</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1672.6306134579916</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2609.2401229112861</v>
+        <v>2608.6793612619822</v>
       </c>
       <c r="B15">
-        <v>2053.9282352566352</v>
+        <v>2053.6014331011174</v>
       </c>
       <c r="C15">
-        <v>1936.1043017785341</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1940.6135712709113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2247.0698900004686</v>
+        <v>2247.0467798670688</v>
       </c>
       <c r="B16">
-        <v>1531.9955049925056</v>
+        <v>1531.9959506533103</v>
       </c>
       <c r="C16">
-        <v>1285.6430914878229</v>
+        <v>1285.6398882655087</v>
       </c>
     </row>
   </sheetData>

</xml_diff>